<commit_message>
docs: customizando o readme
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,357 +453,340 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SKEMA BARRETOS forros, divisórias e vidros</t>
+          <t>CERIMONIAL SHOW</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2055 Rua Brasil</t>
+          <t>Mais de 10 anos no mercado</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(17) 3322-3956</t>
+          <t>Av. Treze, n° 7A</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Fortaleza Da Construção de Barretos LTDA</t>
+          <t>Comitivas - Espaço de Eventos</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Av. 9, 990</t>
+          <t>R. Comitivas, das Dr. Roberto Cardoso Alves, 5038</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(17) 3322-0100</t>
+          <t>(17) 98145-4054</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bodão Materiais para Construção</t>
+          <t>Espaço Magui</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Alameda Líbano, 967</t>
+          <t>Rua CJ10, R. Vitalina Silva Neves, 38</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(17) 3324-3234</t>
+          <t>(17) 98810-6080</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Constru América Materiais de Contrução</t>
+          <t>Espaço Berrantão</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R. Argentina, 2596</t>
+          <t>Rodovia Brigadeiro Faria Lima, km 428, s/n</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(17) 3322-5261</t>
+          <t>Não Informado</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lojao Da Construção</t>
+          <t>Camarote Brahma</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R. Trinta, 048</t>
+          <t>Av. dos bretes, s/n</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(17) 3321-3688</t>
+          <t>(17) 3321-0000</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Constru Ribeiro Com Materiais Construção</t>
+          <t>Barretão Tendas</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Av. Mato Grosso, 695</t>
+          <t>Rua Ibrahim Chehadi</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>(17) 3321-5455</t>
+          <t>(17) 98108-2227</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Trevão Home Center</t>
+          <t>Badalasom - Locação de Geradores Barretos 24h</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Av. dos Maçons, 250</t>
+          <t>(17) 99777-2001</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>(17) 3321-5533</t>
+          <t>Não Informado</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>RIOMAR CONSTRUÇÃO</t>
+          <t>Ramos Vídeo</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R. Messias Gonçalves, 1241</t>
+          <t>Av. Quarenta e Cinco (Numeração Com Zero Inicial), No. 0184</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>(17) 3321-0300</t>
+          <t>(17) 98156-2308</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Comap</t>
+          <t>Nobreza Pulpitos</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Av. 47, 485</t>
+          <t>Av. Onze, 342</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>(17) 3321-0200</t>
+          <t>(17) 98100-0515</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A Construtora</t>
+          <t>Parque do Peão Os Independentes</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R. Trinta, 281</t>
+          <t>Rod. Brg. Faria Lima, Km 428</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>(17) 3322-6533</t>
+          <t>(17) 3321-0000</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>À Construir Materiais de Construção, Elétrico e Hidráulico</t>
+          <t>ESPAÇO DE LAZER BAMBÃ BARRETOS</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R. C- Oito, 181</t>
+          <t>Av. Sf- Um</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>(17) 3312-1081</t>
+          <t>(17) 99226-7578</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ABC da Construção Barretos</t>
+          <t>Doce boutique confeitaria</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R. Vinte e Quatro, 290</t>
+          <t>R. João Luís da Silva</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>(17) 3324-5598</t>
+          <t>(17) 98825-2587</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Constru Center</t>
+          <t>Power Técnica</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Av. António Frederico Ozanam, 1447</t>
+          <t>R. Dez, 187</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>(17) 3323-3229</t>
+          <t>(17) 99112-2009</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>JA Construções e Comércio</t>
+          <t>Fábrica de Salgados</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Av. Trinta e Três, 1350</t>
+          <t>Av. Hércules Brasolin, 339</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>(17) 99773-4441</t>
+          <t>(17) 3322-7775</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Balduino Tijolos e Telhas Barretos</t>
+          <t>Os Independentes</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Av. Brg. Eduardo Gomes, 1585</t>
+          <t>Rod. Brg. Faria Lima, 428</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>(17) 99156-6914</t>
+          <t>(17) 3321-0001</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Preço Bom - Lar e Construção</t>
+          <t>Recinto Paulo de Lima Correa</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Av. MP 17, 802</t>
+          <t>Av. Vinte e Três</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>(17) 98226-5335</t>
+          <t>Não Informado</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ObraNorte Materiais para Construção</t>
+          <t>Trajes Masculinos a Rigor</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R. Venezuela, 2041</t>
+          <t>Av. Vinte e Sete, n 442</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>(17) 98209-9075</t>
+          <t>(17) 99161-3312</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Dos Santos Materiais Para Construção</t>
+          <t>Perfumaria Emy</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>R. Francisco de Assis Martins, 22</t>
+          <t>R. Vinte, 727</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>(17) 3312-9000</t>
+          <t>(17) 3325-7474</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Armazém Lar e Construcão</t>
+          <t>Conka Filmes</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Av. SD 11 - Marcolino Borges, 106</t>
+          <t>(17) 99256-2426</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>(17) 3312-1109</t>
+          <t>Não Informado</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Bento Construções</t>
+          <t>Machado Alfaiate - Costura e Bordados</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Av. Padre Cesar Luzio, 659 - 800</t>
+          <t>Mais de 15 anos no mercado</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>(17) 3325-3066</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>j.senabio construção</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>R. Maria Osório Franco, 361</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Não Informado</t>
+          <t>esquina com a - Av. 9, R. Uruguai, 2681</t>
         </is>
       </c>
     </row>

</xml_diff>